<commit_message>
rename Apple1 to Apple-I and add Apple-II 20211218
</commit_message>
<xml_diff>
--- a/Data Summary.xlsx
+++ b/Data Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\rpt_MiSTer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A09382-ADB3-4BCB-AE95-88EDA1EBA802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE62E86-BD3A-4885-BC93-8FC7FA02F892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{37C2B680-BAE7-40E2-B67E-A259EDFD5F13}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="68">
   <si>
     <t>Core</t>
   </si>
@@ -210,9 +210,6 @@
     <t>34 / 112</t>
   </si>
   <si>
-    <t>AppleI</t>
-  </si>
-  <si>
     <t>7,013 / 41,910</t>
   </si>
   <si>
@@ -223,6 +220,24 @@
   </si>
   <si>
     <t>29 / 112</t>
+  </si>
+  <si>
+    <t>Apple-I</t>
+  </si>
+  <si>
+    <t>Apple-II</t>
+  </si>
+  <si>
+    <t>14,991 / 41,910</t>
+  </si>
+  <si>
+    <t>2,801,490 / 5,662,720</t>
+  </si>
+  <si>
+    <t>362 / 553</t>
+  </si>
+  <si>
+    <t>37 / 112</t>
   </si>
 </sst>
 </file>
@@ -597,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C7B40B3-AA3D-43AE-95BF-373C1FCAAD18}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,13 +800,13 @@
     </row>
     <row r="6" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="4">
+        <v>20211217</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="B6" s="4">
-        <v>20211217</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="D6" s="5">
         <v>0.17</v>
@@ -800,19 +815,19 @@
         <v>9233</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G6" s="5">
         <v>0.25</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I6" s="5">
         <v>0.33</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K6" s="5">
         <v>0.26</v>
@@ -820,217 +835,252 @@
     </row>
     <row r="7" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="4">
+        <v>20211217</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0.36</v>
+      </c>
+      <c r="E7" s="4">
+        <v>17904</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0.49</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0.65</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="K7" s="5">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="4">
-        <v>20211217</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="B8" s="4">
+        <v>20211217</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D8" s="5">
         <v>0.44</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E8" s="4">
         <v>20526</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="5">
+      <c r="G8" s="5">
         <v>0.14000000000000001</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I7" s="5">
+      <c r="I8" s="5">
         <v>0.22</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K8" s="5">
         <v>0.6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="1">
-        <v>20211217</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="3">
-        <v>0.33</v>
-      </c>
-      <c r="E8" s="1">
-        <v>17567</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="3">
-        <v>0.22</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K8" s="3">
-        <v>0.31</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1">
         <v>20211217</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="D9" s="3">
-        <v>0.51</v>
+        <v>0.33</v>
       </c>
       <c r="E9" s="1">
-        <v>28963</v>
+        <v>17567</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="G9" s="3">
-        <v>0.47</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="I9" s="3">
-        <v>0.65</v>
+        <v>0.22</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="K9" s="3">
-        <v>0.41</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1">
         <v>20211217</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="D10" s="3">
-        <v>0.25</v>
+        <v>0.51</v>
       </c>
       <c r="E10" s="1">
-        <v>13220</v>
+        <v>28963</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="G10" s="3">
-        <v>0.15</v>
+        <v>0.47</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="I10" s="3">
-        <v>0.22</v>
+        <v>0.65</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="K10" s="3">
-        <v>0.32</v>
+        <v>0.41</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B11" s="1">
         <v>20211217</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="D11" s="3">
-        <v>0.31</v>
+        <v>0.25</v>
       </c>
       <c r="E11" s="1">
-        <v>16117</v>
+        <v>13220</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="G11" s="3">
-        <v>0.14000000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="I11" s="3">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="K11" s="3">
-        <v>0.35</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1">
+        <v>20211217</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.31</v>
+      </c>
+      <c r="E12" s="1">
+        <v>16117</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.21</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="1">
-        <v>20211217</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="B13" s="1">
+        <v>20211217</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D13" s="3">
         <v>0.71</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E13" s="1">
         <v>30780</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G13" s="3">
         <v>0.23</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I13" s="3">
         <v>0.45</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K13" s="3">
         <v>0.34</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:K11">
-    <sortCondition ref="A8:A11"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:K12">
+    <sortCondition ref="A9:A12"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Aquarius, Arcade-Arkanoid, and Arcade-Asteroids 20211218
</commit_message>
<xml_diff>
--- a/Data Summary.xlsx
+++ b/Data Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\rpt_MiSTer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E87322-AB57-4CF8-8119-AA521DB8658E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EFFAA25-7FAC-4A29-AC15-96D028AA0847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{37C2B680-BAE7-40E2-B67E-A259EDFD5F13}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="85">
   <si>
     <t>Core</t>
   </si>
@@ -262,6 +262,33 @@
   </si>
   <si>
     <t>339 / 553</t>
+  </si>
+  <si>
+    <t>Aquarius</t>
+  </si>
+  <si>
+    <t>Arcade-Arkanoid</t>
+  </si>
+  <si>
+    <t>11,486 / 41,910</t>
+  </si>
+  <si>
+    <t>1,806,290 / 5,662,720</t>
+  </si>
+  <si>
+    <t>240 / 553</t>
+  </si>
+  <si>
+    <t>Arcade-Asteroids</t>
+  </si>
+  <si>
+    <t>8,479 / 41,910</t>
+  </si>
+  <si>
+    <t>2,520,451 / 5,662,720</t>
+  </si>
+  <si>
+    <t>316 / 553</t>
   </si>
 </sst>
 </file>
@@ -636,15 +663,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C7B40B3-AA3D-43AE-95BF-373C1FCAAD18}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="21.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="17.5703125" style="1"/>
+    <col min="1" max="16384" width="21.85546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -964,217 +991,322 @@
     </row>
     <row r="10" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="4">
+        <v>20211218</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0.27</v>
+      </c>
+      <c r="E10" s="4">
+        <v>12600</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0.48</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0.61</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="5">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="4">
+        <v>20211218</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0.27</v>
+      </c>
+      <c r="E11" s="4">
+        <v>17026</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0.32</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I11" s="5">
+        <v>0.43</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K11" s="5">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="4">
+        <v>20211218</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="E12" s="4">
+        <v>10368</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0.45</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="I12" s="5">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="K12" s="5">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B13" s="4">
         <v>20211217</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D13" s="5">
         <v>0.44</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E13" s="4">
         <v>20526</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F13" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G13" s="5">
         <v>0.14000000000000001</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H13" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="5">
+      <c r="I13" s="5">
         <v>0.22</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="J13" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K10" s="5">
+      <c r="K13" s="5">
         <v>0.6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="1">
-        <v>20211217</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0.33</v>
-      </c>
-      <c r="E11" s="1">
-        <v>17567</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="3">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I11" s="3">
-        <v>0.22</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K11" s="3">
-        <v>0.31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="1">
-        <v>20211217</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="3">
-        <v>0.51</v>
-      </c>
-      <c r="E12" s="1">
-        <v>28963</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" s="3">
-        <v>0.47</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I12" s="3">
-        <v>0.65</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K12" s="3">
-        <v>0.41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="1">
-        <v>20211217</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="E13" s="1">
-        <v>13220</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="3">
-        <v>0.15</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" s="3">
-        <v>0.22</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K13" s="3">
-        <v>0.32</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1">
         <v>20211217</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D14" s="3">
-        <v>0.31</v>
+        <v>0.33</v>
       </c>
       <c r="E14" s="1">
-        <v>16117</v>
+        <v>17567</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="G14" s="3">
         <v>0.14000000000000001</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I14" s="3">
-        <v>0.21</v>
+        <v>0.22</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="K14" s="3">
-        <v>0.35</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B15" s="1">
         <v>20211217</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="3">
+        <v>0.51</v>
+      </c>
+      <c r="E15" s="1">
+        <v>28963</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0.47</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K15" s="3">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="1">
+        <v>20211217</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="E16" s="1">
+        <v>13220</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I16" s="3">
+        <v>0.22</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K16" s="3">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="1">
+        <v>20211217</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.31</v>
+      </c>
+      <c r="E17" s="1">
+        <v>16117</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" s="3">
+        <v>0.21</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K17" s="3">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="1">
+        <v>20211217</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D18" s="3">
         <v>0.71</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E18" s="1">
         <v>30780</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G18" s="3">
         <v>0.23</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I18" s="3">
         <v>0.45</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K15" s="3">
+      <c r="K18" s="3">
         <v>0.34</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A11:K14">
-    <sortCondition ref="A11:A14"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A14:K17">
+    <sortCondition ref="A14:A17"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Add multiple Arcade cores and amstrad
</commit_message>
<xml_diff>
--- a/Data Summary.xlsx
+++ b/Data Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\rpt_MiSTer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC27AE71-DD22-4B56-BED7-83632C249579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0622F0-9316-4D36-98E2-8DA8EB4E94D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{37C2B680-BAE7-40E2-B67E-A259EDFD5F13}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="141">
   <si>
     <t>Core</t>
   </si>
@@ -328,6 +328,135 @@
   </si>
   <si>
     <t>41 / 112</t>
+  </si>
+  <si>
+    <t>Amstrad</t>
+  </si>
+  <si>
+    <t>13,748 / 41,910</t>
+  </si>
+  <si>
+    <t>627,843 / 5,662,720</t>
+  </si>
+  <si>
+    <t>91 / 553</t>
+  </si>
+  <si>
+    <t>Arcade-Bagman</t>
+  </si>
+  <si>
+    <t>12,188 / 41,910</t>
+  </si>
+  <si>
+    <t>1,533,394 / 5,662,720</t>
+  </si>
+  <si>
+    <t>208 / 553</t>
+  </si>
+  <si>
+    <t>Arcade-Berzerk</t>
+  </si>
+  <si>
+    <t>9,405 / 41,910</t>
+  </si>
+  <si>
+    <t>683,410 / 5,662,720</t>
+  </si>
+  <si>
+    <t>101 / 553</t>
+  </si>
+  <si>
+    <t>Arcade-BlackWidow</t>
+  </si>
+  <si>
+    <t>12,358 / 41,910</t>
+  </si>
+  <si>
+    <t>2,270,594 / 5,662,720</t>
+  </si>
+  <si>
+    <t>291 / 553</t>
+  </si>
+  <si>
+    <t>Arcade-BombJack</t>
+  </si>
+  <si>
+    <t>15,025 / 41,910</t>
+  </si>
+  <si>
+    <t>1,533,938 / 5,662,720</t>
+  </si>
+  <si>
+    <t>209 / 553</t>
+  </si>
+  <si>
+    <t>Arcade-Breakout</t>
+  </si>
+  <si>
+    <t>8,956 / 41,910</t>
+  </si>
+  <si>
+    <t>463,299 / 5,662,720</t>
+  </si>
+  <si>
+    <t>Arcade-BurgerTime</t>
+  </si>
+  <si>
+    <t>10,929 / 41,910</t>
+  </si>
+  <si>
+    <t>995,330 / 5,662,720</t>
+  </si>
+  <si>
+    <t>140 / 553</t>
+  </si>
+  <si>
+    <t>Arcade-BurningRubber</t>
+  </si>
+  <si>
+    <t>24,592 / 41,910</t>
+  </si>
+  <si>
+    <t>856,226 / 5,662,720</t>
+  </si>
+  <si>
+    <t>125 / 553</t>
+  </si>
+  <si>
+    <t>Arcade-CanyonBomber</t>
+  </si>
+  <si>
+    <t>8,933 / 41,910</t>
+  </si>
+  <si>
+    <t>453,571 / 5,662,720</t>
+  </si>
+  <si>
+    <t>74 / 553</t>
+  </si>
+  <si>
+    <t>Arcade-Centipede</t>
+  </si>
+  <si>
+    <t>17,010 / 41,910</t>
+  </si>
+  <si>
+    <t>509,651 / 5,662,720</t>
+  </si>
+  <si>
+    <t>84 / 553</t>
+  </si>
+  <si>
+    <t>Arcade-ComputerSpace</t>
+  </si>
+  <si>
+    <t>8,508 / 41,910</t>
+  </si>
+  <si>
+    <t>333,427 / 5,662,720</t>
+  </si>
+  <si>
+    <t>52 / 553</t>
   </si>
 </sst>
 </file>
@@ -702,10 +831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C7B40B3-AA3D-43AE-95BF-373C1FCAAD18}">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,136 +1030,136 @@
     </row>
     <row r="6" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>72</v>
+        <v>98</v>
       </c>
       <c r="B6" s="4">
         <v>20211218</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="D6" s="5">
-        <v>0.27</v>
+        <v>0.33</v>
       </c>
       <c r="E6" s="4">
-        <v>12600</v>
+        <v>16587</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="G6" s="5">
-        <v>0.48</v>
+        <v>0.11</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="I6" s="5">
-        <v>0.61</v>
+        <v>0.16</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="K6" s="5">
-        <v>0.32</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="B7" s="4">
-        <v>20211217</v>
+        <v>20211218</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="D7" s="5">
-        <v>0.17</v>
+        <v>0.27</v>
       </c>
       <c r="E7" s="4">
-        <v>9233</v>
+        <v>12600</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="G7" s="5">
-        <v>0.25</v>
+        <v>0.48</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="I7" s="5">
-        <v>0.33</v>
+        <v>0.61</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="K7" s="5">
-        <v>0.26</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" s="4">
-        <v>20211218</v>
+        <v>20211217</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D8" s="5">
-        <v>0.36</v>
+        <v>0.17</v>
       </c>
       <c r="E8" s="4">
-        <v>17904</v>
+        <v>9233</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G8" s="5">
-        <v>0.49</v>
+        <v>0.25</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="I8" s="5">
-        <v>0.65</v>
+        <v>0.33</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="K8" s="5">
-        <v>0.33</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B9" s="4">
         <v>20211218</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D9" s="5">
-        <v>0.23</v>
+        <v>0.36</v>
       </c>
       <c r="E9" s="4">
-        <v>11739</v>
+        <v>17904</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G9" s="5">
-        <v>0.2</v>
+        <v>0.49</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I9" s="5">
-        <v>0.27</v>
+        <v>0.65</v>
       </c>
       <c r="J9" s="4" t="s">
         <v>67</v>
@@ -1041,427 +1170,812 @@
     </row>
     <row r="10" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B10" s="4">
         <v>20211218</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D10" s="5">
+        <v>0.23</v>
+      </c>
+      <c r="E10" s="4">
+        <v>11739</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I10" s="5">
         <v>0.27</v>
       </c>
-      <c r="E10" s="4">
-        <v>12600</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G10" s="5">
-        <v>0.48</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="I10" s="5">
-        <v>0.61</v>
-      </c>
       <c r="J10" s="4" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="K10" s="5">
-        <v>0.32</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B11" s="4">
         <v>20211218</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D11" s="5">
         <v>0.27</v>
       </c>
       <c r="E11" s="4">
-        <v>17026</v>
+        <v>12600</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G11" s="5">
+        <v>0.48</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" s="5">
+        <v>0.61</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K11" s="5">
         <v>0.32</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="I11" s="5">
-        <v>0.43</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="K11" s="5">
-        <v>0.34</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B12" s="4">
         <v>20211218</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D12" s="5">
-        <v>0.2</v>
+        <v>0.27</v>
       </c>
       <c r="E12" s="4">
-        <v>10368</v>
+        <v>17026</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G12" s="5">
-        <v>0.45</v>
+        <v>0.32</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I12" s="5">
-        <v>0.56999999999999995</v>
+        <v>0.43</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="K12" s="5">
-        <v>0.33</v>
+        <v>0.34</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B13" s="4">
         <v>20211218</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D13" s="5">
         <v>0.2</v>
       </c>
       <c r="E13" s="4">
-        <v>10521</v>
+        <v>10368</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G13" s="5">
         <v>0.45</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="I13" s="5">
-        <v>0.57999999999999996</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
       <c r="K13" s="5">
-        <v>0.32</v>
+        <v>0.33</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B14" s="4">
         <v>20211218</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D14" s="5">
-        <v>0.28999999999999998</v>
+        <v>0.2</v>
       </c>
       <c r="E14" s="4">
-        <v>13751</v>
+        <v>10521</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="G14" s="5">
-        <v>0.56000000000000005</v>
+        <v>0.45</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="I14" s="5">
-        <v>0.73</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>97</v>
+        <v>11</v>
       </c>
       <c r="K14" s="5">
-        <v>0.37</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B15" s="4">
         <v>20211218</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D15" s="5">
-        <v>0.22</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="E15" s="4">
-        <v>12755</v>
+        <v>13751</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="G15" s="5">
-        <v>0.28000000000000003</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="I15" s="5">
+        <v>0.73</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="K15" s="5">
         <v>0.37</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="K15" s="5">
-        <v>0.31</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>26</v>
+        <v>89</v>
       </c>
       <c r="B16" s="4">
-        <v>20211217</v>
+        <v>20211218</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="D16" s="5">
-        <v>0.44</v>
+        <v>0.22</v>
       </c>
       <c r="E16" s="4">
-        <v>20526</v>
+        <v>12755</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>28</v>
+        <v>91</v>
       </c>
       <c r="G16" s="5">
-        <v>0.14000000000000001</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>10</v>
+        <v>92</v>
       </c>
       <c r="I16" s="5">
+        <v>0.37</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" s="5">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B17" s="4">
+        <v>20211218</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E17" s="4">
+        <v>16083</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0.27</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="I17" s="5">
+        <v>0.38</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="K17" s="5">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B18" s="4">
+        <v>20211218</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="D18" s="5">
         <v>0.22</v>
       </c>
-      <c r="J16" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K16" s="5">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1">
-        <v>20211217</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="3">
-        <v>0.33</v>
-      </c>
-      <c r="E17" s="1">
-        <v>17567</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="3">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I17" s="3">
-        <v>0.22</v>
-      </c>
-      <c r="J17" s="1" t="s">
+      <c r="E18" s="4">
+        <v>12601</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0.12</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="I18" s="5">
+        <v>0.18</v>
+      </c>
+      <c r="J18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="K17" s="3">
+      <c r="K18" s="5">
         <v>0.31</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B18" s="1">
-        <v>20211217</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="3">
-        <v>0.51</v>
-      </c>
-      <c r="E18" s="1">
-        <v>28963</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G18" s="3">
-        <v>0.47</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I18" s="3">
-        <v>0.65</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K18" s="3">
-        <v>0.41</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B19" s="1">
-        <v>20211217</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="E19" s="1">
-        <v>13220</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G19" s="3">
-        <v>0.15</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I19" s="3">
-        <v>0.22</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K19" s="3">
-        <v>0.32</v>
+    <row r="19" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" s="4">
+        <v>20211218</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E19" s="4">
+        <v>16119</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="G19" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="I19" s="5">
+        <v>0.53</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K19" s="5">
+        <v>0.3</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>21</v>
+        <v>114</v>
       </c>
       <c r="B20" s="1">
-        <v>20211217</v>
+        <v>20211218</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>22</v>
+        <v>115</v>
       </c>
       <c r="D20" s="3">
-        <v>0.31</v>
+        <v>0.36</v>
       </c>
       <c r="E20" s="1">
-        <v>16117</v>
+        <v>18474</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>23</v>
+        <v>116</v>
       </c>
       <c r="G20" s="3">
-        <v>0.14000000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>24</v>
+        <v>117</v>
       </c>
       <c r="I20" s="3">
-        <v>0.21</v>
+        <v>0.38</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="K20" s="3">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21" s="1">
+        <v>20211218</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0.21</v>
+      </c>
+      <c r="E21" s="1">
+        <v>12585</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I21" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K21" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B22" s="1">
+        <v>20211218</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.26</v>
+      </c>
+      <c r="E22" s="1">
+        <v>14857</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0.18</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I22" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K22" s="3">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B23" s="1">
+        <v>20211218</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0.59</v>
+      </c>
+      <c r="E23" s="1">
+        <v>30037</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I23" s="3">
+        <v>0.23</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K23" s="3">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B24" s="1">
+        <v>20211218</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0.21</v>
+      </c>
+      <c r="E24" s="1">
+        <v>11335</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="I24" s="3">
+        <v>0.13</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K24" s="3">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B25" s="1">
+        <v>20211218</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0.41</v>
+      </c>
+      <c r="E25" s="1">
+        <v>28678</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0.09</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="I25" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K25" s="3">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B26" s="1">
+        <v>20211218</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D26" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="E26" s="1">
+        <v>10378</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I26" s="3">
+        <v>0.09</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K26" s="3">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27" s="4">
+        <v>20211217</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="5">
+        <v>0.44</v>
+      </c>
+      <c r="E27" s="4">
+        <v>20526</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G27" s="5">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I27" s="5">
+        <v>0.22</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K27" s="5">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B28" s="1">
+        <v>20211217</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="E28" s="1">
+        <v>17567</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I28" s="3">
+        <v>0.22</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K28" s="3">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="1">
+        <v>20211217</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0.51</v>
+      </c>
+      <c r="E29" s="1">
+        <v>28963</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0.47</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I29" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K29" s="3">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="1">
+        <v>20211217</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="E30" s="1">
+        <v>13220</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I30" s="3">
+        <v>0.22</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K30" s="3">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="1">
+        <v>20211217</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0.31</v>
+      </c>
+      <c r="E31" s="1">
+        <v>16117</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G31" s="3">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I31" s="3">
+        <v>0.21</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K31" s="3">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B32" s="1">
         <v>20211217</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D32" s="3">
         <v>0.71</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E32" s="1">
         <v>30780</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G21" s="3">
+      <c r="G32" s="3">
         <v>0.23</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="H32" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I32" s="3">
         <v>0.45</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="J32" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K21" s="3">
+      <c r="K32" s="3">
         <v>0.34</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A17:K20">
-    <sortCondition ref="A17:A20"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A28:K31">
+    <sortCondition ref="A28:A31"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>